<commit_message>
Fix de imágenes de los paretos
</commit_message>
<xml_diff>
--- a/Implementación/Test 1/decisiones_w1.xlsx
+++ b/Implementación/Test 1/decisiones_w1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCLAMR\OneDrive\OneDrive - MIC\Documents\GitHub\Tesis\Implementación\Test 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06B84542-D4A4-4835-8784-04260326436A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAC577AD-9A84-4C0D-BFDA-76B29215D358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{4AF62623-F908-420B-BDF3-5161762B8528}"/>
   </bookViews>
@@ -35,21 +35,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Var1_1</t>
-  </si>
-  <si>
-    <t>Var1_2</t>
-  </si>
-  <si>
-    <t>Var1_3</t>
-  </si>
-  <si>
-    <t>Var1_4</t>
-  </si>
-  <si>
-    <t>Var1_5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Metodo</t>
+  </si>
+  <si>
+    <t>SMARTER</t>
+  </si>
+  <si>
+    <t>Fuzzy</t>
+  </si>
+  <si>
+    <t>TOPSIS</t>
+  </si>
+  <si>
+    <t>GRA</t>
+  </si>
+  <si>
+    <t>CODAS</t>
+  </si>
+  <si>
+    <t>MABAC</t>
+  </si>
+  <si>
+    <t>VIKOR</t>
+  </si>
+  <si>
+    <t>PROMETHEE II</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Ry</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Entropia</t>
+  </si>
+  <si>
+    <t>SSIM</t>
   </si>
 </sst>
 </file>
@@ -401,166 +428,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE04178-CFA4-4394-A151-25D1CD032D09}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>7.039075411229633</v>
+      </c>
+      <c r="F2">
+        <v>0.99966336549262891</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>278</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.357129793786771E-3</v>
+      </c>
+      <c r="E3">
+        <v>7.3463568259022773</v>
+      </c>
+      <c r="F3">
+        <v>0.9720353030008716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4">
+        <v>108</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>6.840852443555645E-4</v>
+      </c>
+      <c r="E4">
+        <v>7.1960019999241087</v>
+      </c>
+      <c r="F4">
+        <v>0.9905643078314238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>19</v>
-      </c>
-      <c r="C2">
+      <c r="B5">
+        <v>931</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>7.039075411229633</v>
-      </c>
-      <c r="E2">
-        <v>0.99966336549262891</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>278</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1.357129793786771E-3</v>
-      </c>
-      <c r="D3">
-        <v>7.3463568259022773</v>
-      </c>
-      <c r="E3">
-        <v>0.9720353030008716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>108</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>6.840852443555645E-4</v>
-      </c>
-      <c r="D4">
-        <v>7.1960019999241087</v>
-      </c>
-      <c r="E4">
-        <v>0.9905643078314238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E5">
+        <v>7.0624867683220067</v>
+      </c>
+      <c r="F5">
+        <v>0.99886743782409793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>7.0214598057316779</v>
+      </c>
+      <c r="F6">
+        <v>0.99992708330195212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>931</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E7">
         <v>7.0624867683220067</v>
       </c>
-      <c r="E5">
+      <c r="F7">
         <v>0.99886743782409793</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>54</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>931</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>7.0214598057316779</v>
-      </c>
-      <c r="E6">
-        <v>0.99992708330195212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>931</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
+      <c r="E8">
         <v>7.0624867683220067</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>0.99886743782409793</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>931</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>7.0624867683220067</v>
-      </c>
-      <c r="E8">
-        <v>0.99886743782409793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>1.5009022919876269E-3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>7.4034468054930302</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.9706943385677762</v>
       </c>
     </row>

</xml_diff>